<commit_message>
Added data export functionality to .xlxs
</commit_message>
<xml_diff>
--- a/updateOct11/cpu/FCFS.xlsx
+++ b/updateOct11/cpu/FCFS.xlsx
@@ -12,7 +12,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>AVG_QUEUE_SIZE</t>
+  </si>
+  <si>
+    <t>CPU_TIME</t>
+  </si>
+  <si>
+    <t>TURNAROUND</t>
+  </si>
+  <si>
+    <t>WAITCPU_TIME</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,520 +71,537 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="B1" t="n">
-        <v>600.259035986123</v>
-      </c>
-      <c r="C1" t="n">
-        <v>1260.287938248211</v>
-      </c>
-      <c r="D1" t="n">
-        <v>59.76986627596866</v>
-      </c>
-      <c r="E1" t="n">
-        <v>10600.25903598612</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5050.0</v>
+        <v>0.0</v>
       </c>
       <c r="B2" t="n">
-        <v>600.7860724684078</v>
+        <v>600.1786765876939</v>
       </c>
       <c r="C2" t="n">
-        <v>2.650892095513545E7</v>
+        <v>1110.6713147493913</v>
       </c>
       <c r="D2" t="n">
-        <v>2.650771938299057E7</v>
+        <v>-89.68603842599956</v>
       </c>
       <c r="E2" t="n">
-        <v>10600.786072468412</v>
+        <v>10600.178676587622</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>10100.0</v>
+        <v>5050.0</v>
       </c>
       <c r="B3" t="n">
-        <v>600.0269680398304</v>
+        <v>600.2734623154453</v>
       </c>
       <c r="C3" t="n">
-        <v>3.534168396831784E7</v>
+        <v>2.6506780084395435E7</v>
       </c>
       <c r="D3" t="n">
-        <v>3.534048391438197E7</v>
+        <v>2.6505579537470844E7</v>
       </c>
       <c r="E3" t="n">
-        <v>10600.026968039772</v>
+        <v>10600.273462315425</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>15150.0</v>
+        <v>10100.0</v>
       </c>
       <c r="B4" t="n">
-        <v>600.218494846082</v>
+        <v>599.863315877137</v>
       </c>
       <c r="C4" t="n">
-        <v>3.976001640635528E7</v>
+        <v>3.534137164699681E7</v>
       </c>
       <c r="D4" t="n">
-        <v>3.9758815969365686E7</v>
+        <v>3.534017192036523E7</v>
       </c>
       <c r="E4" t="n">
-        <v>10600.218494846084</v>
+        <v>10599.863315877154</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>20200.0</v>
+        <v>15150.0</v>
       </c>
       <c r="B5" t="n">
-        <v>600.385315184126</v>
+        <v>599.8839328579674</v>
       </c>
       <c r="C5" t="n">
-        <v>4.2411378384575136E7</v>
+        <v>3.9758468622583374E7</v>
       </c>
       <c r="D5" t="n">
-        <v>4.241017761394465E7</v>
+        <v>3.975726885471767E7</v>
       </c>
       <c r="E5" t="n">
-        <v>10600.385315184116</v>
+        <v>10599.88393285799</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>25250.0</v>
+        <v>20200.0</v>
       </c>
       <c r="B6" t="n">
-        <v>600.1135140702941</v>
+        <v>599.0294156028956</v>
       </c>
       <c r="C6" t="n">
-        <v>4.41768604228668E7</v>
+        <v>4.240440069224727E7</v>
       </c>
       <c r="D6" t="n">
-        <v>4.417566019583881E7</v>
+        <v>4.2403202633415975E7</v>
       </c>
       <c r="E6" t="n">
-        <v>10600.113514070257</v>
+        <v>10599.029415602874</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>30300.0</v>
+        <v>25250.0</v>
       </c>
       <c r="B7" t="n">
-        <v>600.6431656233062</v>
+        <v>599.722036387929</v>
       </c>
       <c r="C7" t="n">
-        <v>4.5442646267179385E7</v>
+        <v>4.417544745533647E7</v>
       </c>
       <c r="D7" t="n">
-        <v>4.5441444980848245E7</v>
+        <v>4.417424801126365E7</v>
       </c>
       <c r="E7" t="n">
-        <v>10600.643165623282</v>
+        <v>10599.722036387933</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>35350.0</v>
+        <v>30300.0</v>
       </c>
       <c r="B8" t="n">
-        <v>600.090748023648</v>
+        <v>599.8093132651502</v>
       </c>
       <c r="C8" t="n">
-        <v>4.638614646252388E7</v>
+        <v>4.543687634597429E7</v>
       </c>
       <c r="D8" t="n">
-        <v>4.6384946281027846E7</v>
+        <v>4.5435676727347724E7</v>
       </c>
       <c r="E8" t="n">
-        <v>10600.090748023584</v>
+        <v>10599.80931326514</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>40400.0</v>
+        <v>35350.0</v>
       </c>
       <c r="B9" t="n">
-        <v>600.3540425935203</v>
+        <v>601.1618764543401</v>
       </c>
       <c r="C9" t="n">
-        <v>4.712461443332158E7</v>
+        <v>4.638817957135601E7</v>
       </c>
       <c r="D9" t="n">
-        <v>4.712341372523664E7</v>
+        <v>4.6386977247602984E7</v>
       </c>
       <c r="E9" t="n">
-        <v>10600.354042593548</v>
+        <v>10601.161876454347</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>45450.0</v>
+        <v>40400.0</v>
       </c>
       <c r="B10" t="n">
-        <v>599.8214523223465</v>
+        <v>599.9326282787472</v>
       </c>
       <c r="C10" t="n">
-        <v>4.7709084512767754E7</v>
+        <v>4.712024016191907E7</v>
       </c>
       <c r="D10" t="n">
-        <v>4.770788486986321E7</v>
+        <v>4.711904029666239E7</v>
       </c>
       <c r="E10" t="n">
-        <v>10599.821452322334</v>
+        <v>10599.932628278817</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>50500.0</v>
+        <v>45450.0</v>
       </c>
       <c r="B11" t="n">
-        <v>599.7812970424075</v>
+        <v>599.8932595643627</v>
       </c>
       <c r="C11" t="n">
-        <v>4.819108731745147E7</v>
+        <v>4.770867627671787E7</v>
       </c>
       <c r="D11" t="n">
-        <v>4.8189887754857324E7</v>
+        <v>4.770747649019869E7</v>
       </c>
       <c r="E11" t="n">
-        <v>10599.781297042415</v>
+        <v>10599.89325956433</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>55550.0</v>
+        <v>50500.0</v>
       </c>
       <c r="B12" t="n">
-        <v>599.6767563004001</v>
+        <v>599.8356060257429</v>
       </c>
       <c r="C12" t="n">
-        <v>4.859529525407616E7</v>
+        <v>4.819062492878831E7</v>
       </c>
       <c r="D12" t="n">
-        <v>4.8594095900563575E7</v>
+        <v>4.818942525757654E7</v>
       </c>
       <c r="E12" t="n">
-        <v>10599.67675630039</v>
+        <v>10599.835606025727</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>60600.0</v>
+        <v>55550.0</v>
       </c>
       <c r="B13" t="n">
-        <v>600.0368852876389</v>
+        <v>599.8680851702761</v>
       </c>
       <c r="C13" t="n">
-        <v>4.893667195868881E7</v>
+        <v>4.859350625716849E7</v>
       </c>
       <c r="D13" t="n">
-        <v>4.893547188491831E7</v>
+        <v>4.859230652099823E7</v>
       </c>
       <c r="E13" t="n">
-        <v>10600.03688528763</v>
+        <v>10599.868085170252</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>65650.0</v>
+        <v>60600.0</v>
       </c>
       <c r="B14" t="n">
-        <v>600.0773800197447</v>
+        <v>599.2859590374663</v>
       </c>
       <c r="C14" t="n">
-        <v>4.9225874762854956E7</v>
+        <v>4.893100772528842E7</v>
       </c>
       <c r="D14" t="n">
-        <v>4.92246746080951E7</v>
+        <v>4.89298091533702E7</v>
       </c>
       <c r="E14" t="n">
-        <v>10600.077380019724</v>
+        <v>10599.28595903749</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>70700.0</v>
+        <v>65650.0</v>
       </c>
       <c r="B15" t="n">
-        <v>599.7059079339915</v>
+        <v>601.4329534370825</v>
       </c>
       <c r="C15" t="n">
-        <v>4.947532305290558E7</v>
+        <v>4.9233503296558246E7</v>
       </c>
       <c r="D15" t="n">
-        <v>4.947412364108981E7</v>
+        <v>4.923230043065156E7</v>
       </c>
       <c r="E15" t="n">
-        <v>10599.705907934005</v>
+        <v>10601.432953437166</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>75750.0</v>
+        <v>70700.0</v>
       </c>
       <c r="B16" t="n">
-        <v>600.1381021402295</v>
+        <v>600.5477993994089</v>
       </c>
       <c r="C16" t="n">
-        <v>4.970019818862253E7</v>
+        <v>4.9479844527474456E7</v>
       </c>
       <c r="D16" t="n">
-        <v>4.969899791241807E7</v>
+        <v>4.947864343187577E7</v>
       </c>
       <c r="E16" t="n">
-        <v>10600.138102140218</v>
+        <v>10600.547799399383</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>80800.0</v>
+        <v>75750.0</v>
       </c>
       <c r="B17" t="n">
-        <v>599.8368362576545</v>
+        <v>599.5671963203881</v>
       </c>
       <c r="C17" t="n">
-        <v>4.989504017718694E7</v>
+        <v>4.969779921710685E7</v>
       </c>
       <c r="D17" t="n">
-        <v>4.989384050351412E7</v>
+        <v>4.9696600082714215E7</v>
       </c>
       <c r="E17" t="n">
-        <v>10599.836836257644</v>
+        <v>10599.56719632046</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>85850.0</v>
+        <v>80800.0</v>
       </c>
       <c r="B18" t="n">
-        <v>600.2830494761746</v>
+        <v>599.7608156222598</v>
       </c>
       <c r="C18" t="n">
-        <v>5.006720416512136E7</v>
+        <v>4.988909363548438E7</v>
       </c>
       <c r="D18" t="n">
-        <v>5.006600359902227E7</v>
+        <v>4.9887894113853246E7</v>
       </c>
       <c r="E18" t="n">
-        <v>10600.283049476164</v>
+        <v>10599.760815622272</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>90900.0</v>
+        <v>85850.0</v>
       </c>
       <c r="B19" t="n">
-        <v>599.6571235085636</v>
+        <v>600.1295188632702</v>
       </c>
       <c r="C19" t="n">
-        <v>5.022074869348565E7</v>
+        <v>5.0065440677055664E7</v>
       </c>
       <c r="D19" t="n">
-        <v>5.021954937923848E7</v>
+        <v>5.006424041801799E7</v>
       </c>
       <c r="E19" t="n">
-        <v>10599.657123508608</v>
+        <v>10600.129518863296</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>95950.0</v>
+        <v>90900.0</v>
       </c>
       <c r="B20" t="n">
-        <v>600.4438123624363</v>
+        <v>600.8056482179879</v>
       </c>
       <c r="C20" t="n">
-        <v>5.036048113354578E7</v>
+        <v>5.02250679838673E7</v>
       </c>
       <c r="D20" t="n">
-        <v>5.035928024592118E7</v>
+        <v>5.022386637257095E7</v>
       </c>
       <c r="E20" t="n">
-        <v>10600.44381236243</v>
+        <v>10600.805648217995</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>101000.0</v>
+        <v>95950.0</v>
       </c>
       <c r="B21" t="n">
-        <v>600.5676749956749</v>
+        <v>601.022233555583</v>
       </c>
       <c r="C21" t="n">
-        <v>5.0491148043106064E7</v>
+        <v>5.0366436716584966E7</v>
       </c>
       <c r="D21" t="n">
-        <v>5.048994690775625E7</v>
+        <v>5.036523467211791E7</v>
       </c>
       <c r="E21" t="n">
-        <v>10600.567674995715</v>
+        <v>10601.02223355558</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>106050.0</v>
+        <v>101000.0</v>
       </c>
       <c r="B22" t="n">
-        <v>599.6258036215635</v>
+        <v>599.6658017068814</v>
       </c>
       <c r="C22" t="n">
-        <v>5.060104562283489E7</v>
+        <v>5.048609772328191E7</v>
       </c>
       <c r="D22" t="n">
-        <v>5.0599846371227615E7</v>
+        <v>5.0484898391678706E7</v>
       </c>
       <c r="E22" t="n">
-        <v>10599.625803621557</v>
+        <v>10599.66580170689</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>111100.0</v>
+        <v>106050.0</v>
       </c>
       <c r="B23" t="n">
-        <v>599.5522882461945</v>
+        <v>600.0157288637265</v>
       </c>
       <c r="C23" t="n">
-        <v>5.0705460444746904E7</v>
+        <v>5.059920667162721E7</v>
       </c>
       <c r="D23" t="n">
-        <v>5.070426134017022E7</v>
+        <v>5.059800664016957E7</v>
       </c>
       <c r="E23" t="n">
-        <v>10599.552288246216</v>
+        <v>10600.015728863731</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>116150.0</v>
+        <v>111100.0</v>
       </c>
       <c r="B24" t="n">
-        <v>600.0477006390499</v>
+        <v>600.3493921997527</v>
       </c>
       <c r="C24" t="n">
-        <v>5.080254164874885E7</v>
+        <v>5.0709173087948546E7</v>
       </c>
       <c r="D24" t="n">
-        <v>5.080134155334754E7</v>
+        <v>5.070797238916424E7</v>
       </c>
       <c r="E24" t="n">
-        <v>10600.047700639034</v>
+        <v>10600.349392199749</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>121200.0</v>
+        <v>116150.0</v>
       </c>
       <c r="B25" t="n">
-        <v>600.1799083447557</v>
+        <v>600.0934955511588</v>
       </c>
       <c r="C25" t="n">
-        <v>5.089431522101346E7</v>
+        <v>5.080650367510636E7</v>
       </c>
       <c r="D25" t="n">
-        <v>5.089311486119686E7</v>
+        <v>5.080530348811522E7</v>
       </c>
       <c r="E25" t="n">
-        <v>10600.179908344768</v>
+        <v>10600.093495551118</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>126250.0</v>
+        <v>121200.0</v>
       </c>
       <c r="B26" t="n">
-        <v>599.6235682090357</v>
+        <v>600.5978802595424</v>
       </c>
       <c r="C26" t="n">
-        <v>5.097060731171098E7</v>
+        <v>5.089176687172679E7</v>
       </c>
       <c r="D26" t="n">
-        <v>5.0969408064574584E7</v>
+        <v>5.089056567596651E7</v>
       </c>
       <c r="E26" t="n">
-        <v>10599.62356820902</v>
+        <v>10600.597880259567</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>131300.0</v>
+        <v>126250.0</v>
       </c>
       <c r="B27" t="n">
-        <v>599.5106138771175</v>
+        <v>600.454498043545</v>
       </c>
       <c r="C27" t="n">
-        <v>5.104441891789883E7</v>
+        <v>5.0974578932378605E7</v>
       </c>
       <c r="D27" t="n">
-        <v>5.104321989667101E7</v>
+        <v>5.097337802338261E7</v>
       </c>
       <c r="E27" t="n">
-        <v>10599.510613877103</v>
+        <v>10600.454498043558</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>136350.0</v>
+        <v>131300.0</v>
       </c>
       <c r="B28" t="n">
-        <v>599.862117945564</v>
+        <v>599.5562517958011</v>
       </c>
       <c r="C28" t="n">
-        <v>5.1116660731370784E7</v>
+        <v>5.1046085442214444E7</v>
       </c>
       <c r="D28" t="n">
-        <v>5.1115461007134974E7</v>
+        <v>5.104488632971059E7</v>
       </c>
       <c r="E28" t="n">
-        <v>10599.862117945599</v>
+        <v>10599.556251795813</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>141400.0</v>
+        <v>136350.0</v>
       </c>
       <c r="B29" t="n">
-        <v>599.5101728054817</v>
+        <v>599.8702167358459</v>
       </c>
       <c r="C29" t="n">
-        <v>5.118054169470183E7</v>
+        <v>5.111962615091965E7</v>
       </c>
       <c r="D29" t="n">
-        <v>5.117934267435632E7</v>
+        <v>5.111842641048597E7</v>
       </c>
       <c r="E29" t="n">
-        <v>10599.510172805489</v>
+        <v>10599.870216735824</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
+        <v>141400.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>599.6766193999073</v>
+      </c>
+      <c r="C30" t="n">
+        <v>5.118314111228019E7</v>
+      </c>
+      <c r="D30" t="n">
+        <v>5.118194175904146E7</v>
+      </c>
+      <c r="E30" t="n">
+        <v>10599.676619399903</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
         <v>146450.0</v>
       </c>
-      <c r="B30" t="n">
-        <v>599.7272819746707</v>
-      </c>
-      <c r="C30" t="n">
-        <v>5.1243928808991134E7</v>
-      </c>
-      <c r="D30" t="n">
-        <v>5.124272935442688E7</v>
-      </c>
-      <c r="E30" t="n">
-        <v>10599.727281974643</v>
+      <c r="B31" t="n">
+        <v>600.6958945024021</v>
+      </c>
+      <c r="C31" t="n">
+        <v>5.124704045100496E7</v>
+      </c>
+      <c r="D31" t="n">
+        <v>5.1245839059215836E7</v>
+      </c>
+      <c r="E31" t="n">
+        <v>10600.695894502374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned code up some
</commit_message>
<xml_diff>
--- a/updateOct11/cpu/FCFS.xlsx
+++ b/updateOct11/cpu/FCFS.xlsx
@@ -99,16 +99,16 @@
         <v>0.0</v>
       </c>
       <c r="B2" t="n">
-        <v>600.1786765876939</v>
+        <v>599.8753063347568</v>
       </c>
       <c r="C2" t="n">
-        <v>1110.6713147493913</v>
+        <v>1199.7506126695166</v>
       </c>
       <c r="D2" t="n">
-        <v>-89.68603842599956</v>
+        <v>-1.2862974574368025E-12</v>
       </c>
       <c r="E2" t="n">
-        <v>10600.178676587622</v>
+        <v>1199.9353063344545</v>
       </c>
     </row>
     <row r="3">
@@ -116,16 +116,16 @@
         <v>5050.0</v>
       </c>
       <c r="B3" t="n">
-        <v>600.2734623154453</v>
+        <v>599.9678710563109</v>
       </c>
       <c r="C3" t="n">
-        <v>2.6506780084395435E7</v>
+        <v>4502071.385664888</v>
       </c>
       <c r="D3" t="n">
-        <v>2.6505579537470844E7</v>
+        <v>4500871.449922772</v>
       </c>
       <c r="E3" t="n">
-        <v>10600.273462315425</v>
+        <v>1800.0878710555369</v>
       </c>
     </row>
     <row r="4">
@@ -133,16 +133,16 @@
         <v>10100.0</v>
       </c>
       <c r="B4" t="n">
-        <v>599.863315877137</v>
+        <v>600.5594735694418</v>
       </c>
       <c r="C4" t="n">
-        <v>3.534137164699681E7</v>
+        <v>8005255.006019249</v>
       </c>
       <c r="D4" t="n">
-        <v>3.534017192036523E7</v>
+        <v>8004053.887072104</v>
       </c>
       <c r="E4" t="n">
-        <v>10599.863315877154</v>
+        <v>2400.7394735681664</v>
       </c>
     </row>
     <row r="5">
@@ -150,16 +150,16 @@
         <v>15150.0</v>
       </c>
       <c r="B5" t="n">
-        <v>599.8839328579674</v>
+        <v>600.2147822294103</v>
       </c>
       <c r="C5" t="n">
-        <v>3.9758468622583374E7</v>
+        <v>1.12537557173883E7</v>
       </c>
       <c r="D5" t="n">
-        <v>3.975726885471767E7</v>
+        <v>1.1252555287823813E7</v>
       </c>
       <c r="E5" t="n">
-        <v>10599.88393285799</v>
+        <v>3000.4547822276268</v>
       </c>
     </row>
     <row r="6">
@@ -167,16 +167,16 @@
         <v>20200.0</v>
       </c>
       <c r="B6" t="n">
-        <v>599.0294156028956</v>
+        <v>600.3214767115759</v>
       </c>
       <c r="C6" t="n">
-        <v>4.240440069224727E7</v>
+        <v>1.4402697071327845E7</v>
       </c>
       <c r="D6" t="n">
-        <v>4.2403202633415975E7</v>
+        <v>1.4401496428374384E7</v>
       </c>
       <c r="E6" t="n">
-        <v>10599.029415602874</v>
+        <v>3600.6214767092574</v>
       </c>
     </row>
     <row r="7">
@@ -184,16 +184,16 @@
         <v>25250.0</v>
       </c>
       <c r="B7" t="n">
-        <v>599.722036387929</v>
+        <v>600.2360796237413</v>
       </c>
       <c r="C7" t="n">
-        <v>4.417544745533647E7</v>
+        <v>1.75049666031143E7</v>
       </c>
       <c r="D7" t="n">
-        <v>4.417424801126365E7</v>
+        <v>1.750376613095503E7</v>
       </c>
       <c r="E7" t="n">
-        <v>10599.722036387933</v>
+        <v>4200.596079621566</v>
       </c>
     </row>
     <row r="8">
@@ -201,16 +201,16 @@
         <v>30300.0</v>
       </c>
       <c r="B8" t="n">
-        <v>599.8093132651502</v>
+        <v>599.5091579742073</v>
       </c>
       <c r="C8" t="n">
-        <v>4.543687634597429E7</v>
+        <v>2.0573210481114157E7</v>
       </c>
       <c r="D8" t="n">
-        <v>4.5435676727347724E7</v>
+        <v>2.05720114627982E7</v>
       </c>
       <c r="E8" t="n">
-        <v>10599.80931326514</v>
+        <v>4799.929157975466</v>
       </c>
     </row>
     <row r="9">
@@ -218,16 +218,16 @@
         <v>35350.0</v>
       </c>
       <c r="B9" t="n">
-        <v>601.1618764543401</v>
+        <v>599.8249842873151</v>
       </c>
       <c r="C9" t="n">
-        <v>4.638817957135601E7</v>
+        <v>2.3629565619365904E7</v>
       </c>
       <c r="D9" t="n">
-        <v>4.6386977247602984E7</v>
+        <v>2.3628365969397295E7</v>
       </c>
       <c r="E9" t="n">
-        <v>10601.161876454347</v>
+        <v>5400.3049842921855</v>
       </c>
     </row>
     <row r="10">
@@ -235,16 +235,16 @@
         <v>40400.0</v>
       </c>
       <c r="B10" t="n">
-        <v>599.9326282787472</v>
+        <v>600.7954422449061</v>
       </c>
       <c r="C10" t="n">
-        <v>4.712024016191907E7</v>
+        <v>2.6674163092877E7</v>
       </c>
       <c r="D10" t="n">
-        <v>4.711904029666239E7</v>
+        <v>2.66729615019926E7</v>
       </c>
       <c r="E10" t="n">
-        <v>10599.932628278817</v>
+        <v>6001.335442253425</v>
       </c>
     </row>
     <row r="11">
@@ -252,16 +252,16 @@
         <v>45450.0</v>
       </c>
       <c r="B11" t="n">
-        <v>599.8932595643627</v>
+        <v>600.5838988670773</v>
       </c>
       <c r="C11" t="n">
-        <v>4.770867627671787E7</v>
+        <v>2.970826193013732E7</v>
       </c>
       <c r="D11" t="n">
-        <v>4.770747649019869E7</v>
+        <v>2.9707060762339693E7</v>
       </c>
       <c r="E11" t="n">
-        <v>10599.89325956433</v>
+        <v>6601.183898879313</v>
       </c>
     </row>
     <row r="12">
@@ -269,16 +269,16 @@
         <v>50500.0</v>
       </c>
       <c r="B12" t="n">
-        <v>599.8356060257429</v>
+        <v>598.549847177036</v>
       </c>
       <c r="C12" t="n">
-        <v>4.819062492878831E7</v>
+        <v>3.272553490517791E7</v>
       </c>
       <c r="D12" t="n">
-        <v>4.818942525757654E7</v>
+        <v>3.272433780548353E7</v>
       </c>
       <c r="E12" t="n">
-        <v>10599.835606025727</v>
+        <v>7199.209847193052</v>
       </c>
     </row>
     <row r="13">
@@ -286,16 +286,16 @@
         <v>55550.0</v>
       </c>
       <c r="B13" t="n">
-        <v>599.8680851702761</v>
+        <v>599.2015926794934</v>
       </c>
       <c r="C13" t="n">
-        <v>4.859350625716849E7</v>
+        <v>3.5747711194993466E7</v>
       </c>
       <c r="D13" t="n">
-        <v>4.859230652099823E7</v>
+        <v>3.574651279180807E7</v>
       </c>
       <c r="E13" t="n">
-        <v>10599.868085170252</v>
+        <v>7799.921592699312</v>
       </c>
     </row>
     <row r="14">
@@ -303,16 +303,16 @@
         <v>60600.0</v>
       </c>
       <c r="B14" t="n">
-        <v>599.2859590374663</v>
+        <v>601.0588600676085</v>
       </c>
       <c r="C14" t="n">
-        <v>4.893100772528842E7</v>
+        <v>3.87791190586033E7</v>
       </c>
       <c r="D14" t="n">
-        <v>4.89298091533702E7</v>
+        <v>3.877791694088308E7</v>
       </c>
       <c r="E14" t="n">
-        <v>10599.28595903749</v>
+        <v>8401.838860088337</v>
       </c>
     </row>
     <row r="15">
@@ -320,16 +320,16 @@
         <v>65650.0</v>
       </c>
       <c r="B15" t="n">
-        <v>601.4329534370825</v>
+        <v>600.3978231610255</v>
       </c>
       <c r="C15" t="n">
-        <v>4.9233503296558246E7</v>
+        <v>4.179160727100982E7</v>
       </c>
       <c r="D15" t="n">
-        <v>4.923230043065156E7</v>
+        <v>4.179040647536355E7</v>
       </c>
       <c r="E15" t="n">
-        <v>10601.432953437166</v>
+        <v>9001.237823177104</v>
       </c>
     </row>
     <row r="16">
@@ -337,16 +337,16 @@
         <v>70700.0</v>
       </c>
       <c r="B16" t="n">
-        <v>600.5477993994089</v>
+        <v>600.7257533291081</v>
       </c>
       <c r="C16" t="n">
-        <v>4.9479844527474456E7</v>
+        <v>4.4805559540888086E7</v>
       </c>
       <c r="D16" t="n">
-        <v>4.947864343187577E7</v>
+        <v>4.480435808938161E7</v>
       </c>
       <c r="E16" t="n">
-        <v>10600.547799399383</v>
+        <v>9601.625753340439</v>
       </c>
     </row>
     <row r="17">
@@ -354,16 +354,16 @@
         <v>75750.0</v>
       </c>
       <c r="B17" t="n">
-        <v>599.5671963203881</v>
+        <v>599.9898066040677</v>
       </c>
       <c r="C17" t="n">
-        <v>4.969779921710685E7</v>
+        <v>4.781809477343345E7</v>
       </c>
       <c r="D17" t="n">
-        <v>4.9696600082714215E7</v>
+        <v>4.781689479382014E7</v>
       </c>
       <c r="E17" t="n">
-        <v>10599.56719632046</v>
+        <v>10200.94980661068</v>
       </c>
     </row>
     <row r="18">
@@ -371,16 +371,16 @@
         <v>80800.0</v>
       </c>
       <c r="B18" t="n">
-        <v>599.7608156222598</v>
+        <v>600.947707503187</v>
       </c>
       <c r="C18" t="n">
-        <v>4.988909363548438E7</v>
+        <v>5.0832537625580296E7</v>
       </c>
       <c r="D18" t="n">
-        <v>4.9887894113853246E7</v>
+        <v>5.083133573016523E7</v>
       </c>
       <c r="E18" t="n">
-        <v>10599.760815622272</v>
+        <v>10801.967707504975</v>
       </c>
     </row>
     <row r="19">
@@ -388,16 +388,16 @@
         <v>85850.0</v>
       </c>
       <c r="B19" t="n">
-        <v>600.1295188632702</v>
+        <v>600.2994969805065</v>
       </c>
       <c r="C19" t="n">
-        <v>5.0065440677055664E7</v>
+        <v>5.384198996946201E7</v>
       </c>
       <c r="D19" t="n">
-        <v>5.006424041801799E7</v>
+        <v>5.384078937046812E7</v>
       </c>
       <c r="E19" t="n">
-        <v>10600.129518863296</v>
+        <v>11401.379496977459</v>
       </c>
     </row>
     <row r="20">
@@ -405,16 +405,16 @@
         <v>90900.0</v>
       </c>
       <c r="B20" t="n">
-        <v>600.8056482179879</v>
+        <v>600.3554481919007</v>
       </c>
       <c r="C20" t="n">
-        <v>5.02250679838673E7</v>
+        <v>5.685184182696036E7</v>
       </c>
       <c r="D20" t="n">
-        <v>5.022386637257095E7</v>
+        <v>5.685064111606393E7</v>
       </c>
       <c r="E20" t="n">
-        <v>10600.805648217995</v>
+        <v>12001.495448184049</v>
       </c>
     </row>
     <row r="21">
@@ -422,16 +422,16 @@
         <v>95950.0</v>
       </c>
       <c r="B21" t="n">
-        <v>601.022233555583</v>
+        <v>599.5321962735959</v>
       </c>
       <c r="C21" t="n">
-        <v>5.0366436716584966E7</v>
+        <v>5.985278381603763E7</v>
       </c>
       <c r="D21" t="n">
-        <v>5.036523467211791E7</v>
+        <v>5.98515847516452E7</v>
       </c>
       <c r="E21" t="n">
-        <v>10601.02223355558</v>
+        <v>12600.732196260875</v>
       </c>
     </row>
     <row r="22">
@@ -439,16 +439,16 @@
         <v>101000.0</v>
       </c>
       <c r="B22" t="n">
-        <v>599.6658017068814</v>
+        <v>600.5676358301349</v>
       </c>
       <c r="C22" t="n">
-        <v>5.048609772328191E7</v>
+        <v>6.286993014398665E7</v>
       </c>
       <c r="D22" t="n">
-        <v>5.0484898391678706E7</v>
+        <v>6.286872900871471E7</v>
       </c>
       <c r="E22" t="n">
-        <v>10599.66580170689</v>
+        <v>13201.827635812604</v>
       </c>
     </row>
     <row r="23">
@@ -456,16 +456,16 @@
         <v>106050.0</v>
       </c>
       <c r="B23" t="n">
-        <v>600.0157288637265</v>
+        <v>600.8865592689846</v>
       </c>
       <c r="C23" t="n">
-        <v>5.059920667162721E7</v>
+        <v>6.587645928992207E7</v>
       </c>
       <c r="D23" t="n">
-        <v>5.059800664016957E7</v>
+        <v>6.587525751680335E7</v>
       </c>
       <c r="E23" t="n">
-        <v>10600.015728863731</v>
+        <v>13802.20655924644</v>
       </c>
     </row>
     <row r="24">
@@ -473,16 +473,16 @@
         <v>111100.0</v>
       </c>
       <c r="B24" t="n">
-        <v>600.3493921997527</v>
+        <v>598.3720865252427</v>
       </c>
       <c r="C24" t="n">
-        <v>5.0709173087948546E7</v>
+        <v>6.887117498992705E7</v>
       </c>
       <c r="D24" t="n">
-        <v>5.070797238916424E7</v>
+        <v>6.88699782457542E7</v>
       </c>
       <c r="E24" t="n">
-        <v>10600.349392199749</v>
+        <v>14399.752086497885</v>
       </c>
     </row>
     <row r="25">
@@ -490,16 +490,16 @@
         <v>116150.0</v>
       </c>
       <c r="B25" t="n">
-        <v>600.0934955511588</v>
+        <v>600.3936393425197</v>
       </c>
       <c r="C25" t="n">
-        <v>5.080650367510636E7</v>
+        <v>7.18839890505184E7</v>
       </c>
       <c r="D25" t="n">
-        <v>5.080530348811522E7</v>
+        <v>7.188278826323967E7</v>
       </c>
       <c r="E25" t="n">
-        <v>10600.093495551118</v>
+        <v>15001.833639310173</v>
       </c>
     </row>
     <row r="26">
@@ -507,16 +507,16 @@
         <v>121200.0</v>
       </c>
       <c r="B26" t="n">
-        <v>600.5978802595424</v>
+        <v>600.7450952211633</v>
       </c>
       <c r="C26" t="n">
-        <v>5.089176687172679E7</v>
+        <v>7.488920171028914E7</v>
       </c>
       <c r="D26" t="n">
-        <v>5.089056567596651E7</v>
+        <v>7.48880002200993E7</v>
       </c>
       <c r="E26" t="n">
-        <v>10600.597880259567</v>
+        <v>15602.2450951839</v>
       </c>
     </row>
     <row r="27">
@@ -524,16 +524,16 @@
         <v>126250.0</v>
       </c>
       <c r="B27" t="n">
-        <v>600.454498043545</v>
+        <v>599.0875700502468</v>
       </c>
       <c r="C27" t="n">
-        <v>5.0974578932378605E7</v>
+        <v>7.788706059693499E7</v>
       </c>
       <c r="D27" t="n">
-        <v>5.097337802338261E7</v>
+        <v>7.78858624217948E7</v>
       </c>
       <c r="E27" t="n">
-        <v>10600.454498043558</v>
+        <v>16200.647570007946</v>
       </c>
     </row>
     <row r="28">
@@ -541,16 +541,16 @@
         <v>131300.0</v>
       </c>
       <c r="B28" t="n">
-        <v>599.5562517958011</v>
+        <v>600.3245311557905</v>
       </c>
       <c r="C28" t="n">
-        <v>5.1046085442214444E7</v>
+        <v>8.090026282426457E7</v>
       </c>
       <c r="D28" t="n">
-        <v>5.104488632971059E7</v>
+        <v>8.089906217520209E7</v>
       </c>
       <c r="E28" t="n">
-        <v>10599.556251795813</v>
+        <v>16801.944531120753</v>
       </c>
     </row>
     <row r="29">
@@ -558,16 +558,16 @@
         <v>136350.0</v>
       </c>
       <c r="B29" t="n">
-        <v>599.8702167358459</v>
+        <v>598.4569552037689</v>
       </c>
       <c r="C29" t="n">
-        <v>5.111962615091965E7</v>
+        <v>8.389365502980562E7</v>
       </c>
       <c r="D29" t="n">
-        <v>5.111842641048597E7</v>
+        <v>8.389245811589517E7</v>
       </c>
       <c r="E29" t="n">
-        <v>10599.870216735824</v>
+        <v>17400.13695518133</v>
       </c>
     </row>
     <row r="30">
@@ -575,16 +575,16 @@
         <v>141400.0</v>
       </c>
       <c r="B30" t="n">
-        <v>599.6766193999073</v>
+        <v>599.9624324929807</v>
       </c>
       <c r="C30" t="n">
-        <v>5.118314111228019E7</v>
+        <v>8.690780793840191E7</v>
       </c>
       <c r="D30" t="n">
-        <v>5.118194175904146E7</v>
+        <v>8.690660801353706E7</v>
       </c>
       <c r="E30" t="n">
-        <v>10599.676619399903</v>
+        <v>18001.702432483216</v>
       </c>
     </row>
     <row r="31">
@@ -592,16 +592,16 @@
         <v>146450.0</v>
       </c>
       <c r="B31" t="n">
-        <v>600.6958945024021</v>
+        <v>599.7492341130744</v>
       </c>
       <c r="C31" t="n">
-        <v>5.124704045100496E7</v>
+        <v>8.991334390883328E7</v>
       </c>
       <c r="D31" t="n">
-        <v>5.1245839059215836E7</v>
+        <v>8.991214441036497E7</v>
       </c>
       <c r="E31" t="n">
-        <v>10600.695894502374</v>
+        <v>18601.549234115864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>